<commit_message>
Removed major lineage designation from sequence KY586818
</commit_message>
<xml_diff>
--- a/tabular/yale-taxdata-denv3.xlsx
+++ b/tabular/yale-taxdata-denv3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/arbovirus/Dengue-GLUE-Lineages/tabular/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/arbovirus/Dengue/Dengue-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5D4D98-F60D-2044-AB68-C71C275E4916}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE02371D-F306-864C-BA4F-08BA606E91E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="1500" windowWidth="26740" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1291,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1733,7 +1733,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
         <v>3</v>

</xml_diff>